<commit_message>
Arrumei a classificação de alguns tweets
</commit_message>
<xml_diff>
--- a/pepsi.xlsx
+++ b/pepsi.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dom Ruan\2° Semestre Eng\C.Dados\Projeto_1_CDados\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5FB8C88D-5B2B-4792-9444-83A58E579F5E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13E702E0-E0C5-4A37-A044-C370F1250B78}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1795,16 +1795,8 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -1870,19 +1862,16 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="top"/>
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
@@ -2224,9 +2213,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B301"/>
+  <dimension ref="A1:B303"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -2235,7 +2226,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
@@ -2283,11 +2274,11 @@
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
+      <c r="A7" s="2" t="s">
         <v>6</v>
       </c>
       <c r="B7">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
@@ -2303,7 +2294,7 @@
         <v>8</v>
       </c>
       <c r="B9">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.3">
@@ -2323,7 +2314,7 @@
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
+      <c r="A12" s="2" t="s">
         <v>11</v>
       </c>
       <c r="B12">
@@ -2407,7 +2398,7 @@
         <v>21</v>
       </c>
       <c r="B22">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.3">
@@ -2575,7 +2566,7 @@
         <v>42</v>
       </c>
       <c r="B43">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.3">
@@ -2607,7 +2598,7 @@
         <v>46</v>
       </c>
       <c r="B47">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.3">
@@ -2671,7 +2662,7 @@
         <v>54</v>
       </c>
       <c r="B55">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.3">
@@ -3047,7 +3038,7 @@
         <v>101</v>
       </c>
       <c r="B102">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="103" spans="1:2" x14ac:dyDescent="0.3">
@@ -3383,7 +3374,7 @@
         <v>143</v>
       </c>
       <c r="B144">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="145" spans="1:2" x14ac:dyDescent="0.3">
@@ -3575,7 +3566,7 @@
         <v>167</v>
       </c>
       <c r="B168">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="169" spans="1:2" x14ac:dyDescent="0.3">
@@ -3671,7 +3662,7 @@
         <v>179</v>
       </c>
       <c r="B180">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="181" spans="1:2" x14ac:dyDescent="0.3">
@@ -3999,7 +3990,7 @@
         <v>220</v>
       </c>
       <c r="B221">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="222" spans="1:2" x14ac:dyDescent="0.3">
@@ -4023,7 +4014,7 @@
         <v>223</v>
       </c>
       <c r="B224">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="225" spans="1:2" x14ac:dyDescent="0.3">
@@ -4143,7 +4134,7 @@
         <v>238</v>
       </c>
       <c r="B239">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="240" spans="1:2" x14ac:dyDescent="0.3">
@@ -4151,7 +4142,7 @@
         <v>239</v>
       </c>
       <c r="B240">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="241" spans="1:2" x14ac:dyDescent="0.3">
@@ -4231,7 +4222,7 @@
         <v>249</v>
       </c>
       <c r="B250">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="251" spans="1:2" x14ac:dyDescent="0.3">
@@ -4641,6 +4632,9 @@
       <c r="B301">
         <v>0</v>
       </c>
+    </row>
+    <row r="303" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A303" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -4652,8 +4646,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:C201"/>
   <sheetViews>
-    <sheetView topLeftCell="A174" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A202" sqref="A202"/>
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4663,13 +4657,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="3" t="s">
         <v>301</v>
       </c>
       <c r="B1" t="s">
         <v>502</v>
       </c>
-      <c r="C1" s="3"/>
+      <c r="C1" s="2"/>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
@@ -6136,7 +6130,7 @@
       </c>
     </row>
     <row r="185" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A185" s="2" t="s">
+      <c r="A185" s="1" t="s">
         <v>485</v>
       </c>
       <c r="B185">

</xml_diff>